<commit_message>
RSA 1024 2048 性能测试
</commit_message>
<xml_diff>
--- a/src/main/resources/static/xls/TT.xlsx
+++ b/src/main/resources/static/xls/TT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="390" windowWidth="23250" windowHeight="12000"/>
+    <workbookView xWindow="720" yWindow="396" windowWidth="23256" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1972" uniqueCount="1651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="1671">
   <si>
     <t>date</t>
   </si>
@@ -4755,660 +4755,11 @@
     <t>5-九鼎新材-002201.SZ-实体-江苏-34.0</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>正例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>金力永磁 银河磁体 同属一个题材 金力永磁是龙头</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>前一个龙头潜能恒信当天18个点大面 谨慎</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>涨停价开盘|连续3个一字</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>前一个龙头华讯方舟15个点大面 谨慎</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>前一个龙头泰晶科技18个点以上大面，隔天跌停开盘 谨慎</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">涨停价开盘 </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>前一个龙头森远股份18个点以上大面 谨慎</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>前一个龙头宝德股份跌停且隔日竞价低开破5日线 谨慎</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>前一个龙头一拖股份跌停且隔日竞价低开破5日线 谨慎</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>连续3个一字 未破板 不买 筹码断层严重 没换手</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>近两个月最高板无法突破8板 连杀[7-6-5-4]5连杀 没换手</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>涨停价开盘</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>有减持利空的股票排除掉 
-直接找人气最好的下一只 兰石重装</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>有减持利空的股票排除掉 
-直接找人气最好的下一只 铭普光磁</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>正例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>换手 人气好</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>有减持利空的股票排除掉 
-直接找人气最好的下一只 金力永磁</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>6-天龙光电-300029.SZ-非实体-江苏-20.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>6-实达集团-600734.SH-非实体-福建-10.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>前一个龙头实达集团跌停且隔日竞价低开破5日线 谨慎</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>连续3个一字以上 未破板 不买 筹码断层严重 没换手</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>筹码断层严重 没换手</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>正例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>人气足 筹码交换充分 充分换</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>手</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>全是一字板上来 中间没有换手过 筹码断层严重</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>东北+涨停价开盘</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>连续3个一字以上 未破板 不买</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>反例：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>缩量上涨 筹码断层 没经过爆量的考验</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -5570,43 +4921,6 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>反例</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>：</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>缩量(小票) 筹码断层 没换手</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>反例：</t>
     </r>
     <r>
@@ -5820,6 +5134,211 @@
   </si>
   <si>
     <t>3-鲁商发展-600223.SH-非实体-山东-5.0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>反例：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>缩量一字板 没换手 真正龙头是诚迈科技 并架的票 选择低开的</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行情刚起步加分 缩量减分 开盘价4%个多点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 开盘价不高加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前个龙头国风锁业大面泛起</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 低开加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 开盘价在5%左右加分 相比其他并驾的票 位置合适</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 开盘价位置不高加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 水下低开加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>问题股</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择复旦复华 放量加分比国电好 隔日水下大幅低开加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩量减分 前个龙头复旦复华大面放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩量减分 水下开盘加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 水平价附件开盘加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩量减分 水下开盘加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东风科技大面放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东北票减分 涨停价开盘放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>涨停价开盘放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 低开减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩量减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩量减分 开盘价太高减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续3个一字以上 未破板 不买 筹码断层严重 没换手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前一个龙头实达集团跌停且隔日竞价低开破5日线 放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有减持利空的股票排除掉 
+直接找人气最好的下一只 金力永磁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩量减分 高开减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 4%左右开盘加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有减持利空的股票排除掉 
+直接找人气最好的下一只 铭普光磁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有减持利空的股票排除掉 
+直接找人气最好的下一只 兰石重装</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行情起步加分 缩量减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>涨停价开盘放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续3个一字 未破板 不买 筹码断层严重 没换手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩量太厉害减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">涨停价开盘 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前龙森远大面放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前龙宝德大面放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前龙一拖大面放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前龙泰晶科技大面放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放量加分 行情起步加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩量减分 高开太高减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>涨停价开盘|连续3个一字放弃 缩量减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前龙头潜能恒信当天18个点大面放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行情起步加分 缩量减分 实体加分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前一个龙头华讯方舟15个点大面放弃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金力永磁 银河磁体 同属一个题材 金力永磁是龙头</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>行情起步加分 缩量加分 T叠加一字减分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6464,7 +5983,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6513,9 +6032,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -6539,6 +6055,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -6921,22 +6446,22 @@
   <dimension ref="A1:AN512"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A417" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F431" sqref="F431"/>
+      <pane ySplit="1" topLeftCell="A391" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H414" sqref="H414"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="70.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="35.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -20781,6 +20306,9 @@
       <c r="D272" t="s">
         <v>266</v>
       </c>
+      <c r="H272" s="25" t="s">
+        <v>1627</v>
+      </c>
       <c r="I272" t="s">
         <v>1464</v>
       </c>
@@ -21079,6 +20607,9 @@
         <f>(F281-E281)/E281*100</f>
         <v>17.142857142857132</v>
       </c>
+      <c r="H281" s="25" t="s">
+        <v>1628</v>
+      </c>
       <c r="I281" t="s">
         <v>1473</v>
       </c>
@@ -21141,6 +20672,9 @@
         <f t="shared" si="12"/>
         <v>12.023898431665417</v>
       </c>
+      <c r="H283" s="24" t="s">
+        <v>1629</v>
+      </c>
       <c r="I283" t="s">
         <v>1475</v>
       </c>
@@ -21219,6 +20753,9 @@
         <f t="shared" si="12"/>
         <v>83.852691218130332</v>
       </c>
+      <c r="H285" s="25" t="s">
+        <v>1630</v>
+      </c>
       <c r="I285" t="s">
         <v>1477</v>
       </c>
@@ -21258,6 +20795,9 @@
         <f t="shared" si="12"/>
         <v>52.762803234501362</v>
       </c>
+      <c r="H286" s="25" t="s">
+        <v>1631</v>
+      </c>
       <c r="I286" t="s">
         <v>1478</v>
       </c>
@@ -21412,6 +20952,9 @@
         <f t="shared" si="12"/>
         <v>9.5625000000000071</v>
       </c>
+      <c r="H292" s="25" t="s">
+        <v>1632</v>
+      </c>
       <c r="I292" t="s">
         <v>1298</v>
       </c>
@@ -21451,6 +20994,9 @@
         <f t="shared" si="12"/>
         <v>-4.5000000000000036</v>
       </c>
+      <c r="H293" s="24" t="s">
+        <v>1634</v>
+      </c>
       <c r="I293" t="s">
         <v>1480</v>
       </c>
@@ -21513,6 +21059,9 @@
         <f t="shared" si="12"/>
         <v>13.749999999999996</v>
       </c>
+      <c r="H295" s="25" t="s">
+        <v>1633</v>
+      </c>
       <c r="I295" t="s">
         <v>1299</v>
       </c>
@@ -21591,6 +21140,9 @@
         <f t="shared" si="12"/>
         <v>2.1479713603818578</v>
       </c>
+      <c r="H297" s="25" t="s">
+        <v>1635</v>
+      </c>
       <c r="I297" t="s">
         <v>1301</v>
       </c>
@@ -21692,6 +21244,9 @@
         <f t="shared" si="12"/>
         <v>5.26315789473683</v>
       </c>
+      <c r="H300" s="24" t="s">
+        <v>1636</v>
+      </c>
       <c r="I300" t="s">
         <v>1304</v>
       </c>
@@ -21770,6 +21325,9 @@
         <f t="shared" si="12"/>
         <v>10.169491525423737</v>
       </c>
+      <c r="H302" s="25" t="s">
+        <v>1633</v>
+      </c>
       <c r="I302" t="s">
         <v>1306</v>
       </c>
@@ -21809,6 +21367,9 @@
         <f t="shared" si="12"/>
         <v>18.945868945868948</v>
       </c>
+      <c r="H303" s="25" t="s">
+        <v>1633</v>
+      </c>
       <c r="I303" t="s">
         <v>1307</v>
       </c>
@@ -21937,6 +21498,9 @@
         <f>(F307-E307)/E307*100</f>
         <v>2.4287222808869973</v>
       </c>
+      <c r="H307" s="25" t="s">
+        <v>1628</v>
+      </c>
       <c r="I307" t="s">
         <v>1311</v>
       </c>
@@ -21976,6 +21540,9 @@
         <f t="shared" si="12"/>
         <v>-3.8922155688622673</v>
       </c>
+      <c r="H308" s="24" t="s">
+        <v>1637</v>
+      </c>
       <c r="I308" t="s">
         <v>1312</v>
       </c>
@@ -22015,6 +21582,9 @@
         <f t="shared" si="12"/>
         <v>7.5268817204301026</v>
       </c>
+      <c r="H309" s="25" t="s">
+        <v>1638</v>
+      </c>
       <c r="I309" t="s">
         <v>1313</v>
       </c>
@@ -22093,8 +21663,8 @@
         <f t="shared" si="12"/>
         <v>-3.4482758620689689</v>
       </c>
-      <c r="H311" s="14" t="s">
-        <v>1599</v>
+      <c r="H311" s="24" t="s">
+        <v>1639</v>
       </c>
       <c r="I311" t="s">
         <v>1315</v>
@@ -22158,6 +21728,9 @@
         <f t="shared" si="12"/>
         <v>-2.4390243902438939</v>
       </c>
+      <c r="H313" s="24" t="s">
+        <v>1637</v>
+      </c>
       <c r="I313" t="s">
         <v>1317</v>
       </c>
@@ -22187,8 +21760,8 @@
       <c r="D314" t="s">
         <v>308</v>
       </c>
-      <c r="H314" s="15" t="s">
-        <v>1598</v>
+      <c r="H314" s="24" t="s">
+        <v>1521</v>
       </c>
       <c r="I314" t="s">
         <v>1318</v>
@@ -22263,6 +21836,9 @@
         <f t="shared" si="12"/>
         <v>10.134739308728765</v>
       </c>
+      <c r="H317" s="25" t="s">
+        <v>1638</v>
+      </c>
       <c r="O317">
         <v>20170523</v>
       </c>
@@ -22313,6 +21889,9 @@
         <f t="shared" si="12"/>
         <v>12.408759124087593</v>
       </c>
+      <c r="H319" s="24" t="s">
+        <v>1640</v>
+      </c>
       <c r="O319">
         <v>20170525</v>
       </c>
@@ -22343,6 +21922,9 @@
         <f t="shared" si="12"/>
         <v>10.114068441064639</v>
       </c>
+      <c r="H320" s="25" t="s">
+        <v>1638</v>
+      </c>
       <c r="O320">
         <v>20170526</v>
       </c>
@@ -22383,8 +21965,8 @@
       <c r="D322" t="s">
         <v>1489</v>
       </c>
-      <c r="H322" s="15" t="s">
-        <v>1597</v>
+      <c r="H322" s="24" t="s">
+        <v>1641</v>
       </c>
       <c r="O322">
         <v>20170601</v>
@@ -22506,6 +22088,9 @@
       <c r="D328" t="s">
         <v>1495</v>
       </c>
+      <c r="H328" s="24" t="s">
+        <v>1642</v>
+      </c>
       <c r="O328">
         <v>20170609</v>
       </c>
@@ -22536,6 +22121,9 @@
         <f t="shared" ref="G329:G391" si="14">(F329-E329)/E329*100</f>
         <v>2.6622296173044946</v>
       </c>
+      <c r="H329" s="25" t="s">
+        <v>1643</v>
+      </c>
       <c r="O329">
         <v>20170612</v>
       </c>
@@ -22616,6 +22204,9 @@
         <f t="shared" si="14"/>
         <v>3.0303030303030365</v>
       </c>
+      <c r="H332" s="24" t="s">
+        <v>1644</v>
+      </c>
       <c r="O332">
         <v>20170615</v>
       </c>
@@ -22636,6 +22227,9 @@
       <c r="D333" t="s">
         <v>1500</v>
       </c>
+      <c r="H333" s="25" t="s">
+        <v>1638</v>
+      </c>
       <c r="O333">
         <v>20170616</v>
       </c>
@@ -22716,6 +22310,9 @@
         <f t="shared" si="14"/>
         <v>10.140093395597074</v>
       </c>
+      <c r="H336" s="25" t="s">
+        <v>1638</v>
+      </c>
       <c r="O336">
         <v>20170621</v>
       </c>
@@ -22756,6 +22353,9 @@
       <c r="D338" t="s">
         <v>1505</v>
       </c>
+      <c r="H338" s="24" t="s">
+        <v>1645</v>
+      </c>
       <c r="O338">
         <v>20170623</v>
       </c>
@@ -22794,7 +22394,7 @@
         <v>9</v>
       </c>
       <c r="D340" s="13" t="s">
-        <v>1590</v>
+        <v>1574</v>
       </c>
       <c r="E340">
         <v>9.76</v>
@@ -22806,9 +22406,7 @@
         <f t="shared" si="14"/>
         <v>-12.704918032786889</v>
       </c>
-      <c r="H340" s="14" t="s">
-        <v>1594</v>
-      </c>
+      <c r="H340" s="14"/>
       <c r="O340">
         <v>20170627</v>
       </c>
@@ -22827,10 +22425,10 @@
         <v>10</v>
       </c>
       <c r="D341" s="13" t="s">
-        <v>1591</v>
-      </c>
-      <c r="H341" s="15" t="s">
-        <v>1593</v>
+        <v>1575</v>
+      </c>
+      <c r="H341" s="24" t="s">
+        <v>1646</v>
       </c>
       <c r="O341">
         <v>20170628</v>
@@ -22852,8 +22450,8 @@
       <c r="D342" t="s">
         <v>1507</v>
       </c>
-      <c r="H342" s="15" t="s">
-        <v>1592</v>
+      <c r="H342" s="24" t="s">
+        <v>1647</v>
       </c>
       <c r="O342">
         <v>20170629</v>
@@ -22862,7 +22460,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="343" spans="1:16" ht="27">
+    <row r="343" spans="1:16" ht="28.8">
       <c r="A343">
         <v>20190527</v>
       </c>
@@ -22875,8 +22473,8 @@
       <c r="D343" t="s">
         <v>1508</v>
       </c>
-      <c r="H343" s="16" t="s">
-        <v>1589</v>
+      <c r="H343" s="26" t="s">
+        <v>1648</v>
       </c>
       <c r="O343">
         <v>20170630</v>
@@ -22928,6 +22526,9 @@
         <f t="shared" si="14"/>
         <v>-3.7565973300217346</v>
       </c>
+      <c r="H345" s="24" t="s">
+        <v>1649</v>
+      </c>
       <c r="O345">
         <v>20170704</v>
       </c>
@@ -22958,6 +22559,9 @@
         <f t="shared" si="14"/>
         <v>9.0014064697608944</v>
       </c>
+      <c r="H346" s="25" t="s">
+        <v>1650</v>
+      </c>
       <c r="O346">
         <v>20170705</v>
       </c>
@@ -22985,7 +22589,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="348" spans="1:16" ht="27">
+    <row r="348" spans="1:16" ht="28.8">
       <c r="A348">
         <v>20190603</v>
       </c>
@@ -22998,8 +22602,8 @@
       <c r="D348" t="s">
         <v>1513</v>
       </c>
-      <c r="H348" s="16" t="s">
-        <v>1587</v>
+      <c r="H348" s="26" t="s">
+        <v>1651</v>
       </c>
       <c r="O348">
         <v>20170707</v>
@@ -23031,8 +22635,8 @@
         <f t="shared" si="14"/>
         <v>1.0356150543066343</v>
       </c>
-      <c r="H349" s="14" t="s">
-        <v>1595</v>
+      <c r="H349" s="25" t="s">
+        <v>1628</v>
       </c>
       <c r="O349">
         <v>20170710</v>
@@ -23084,6 +22688,9 @@
         <f t="shared" si="14"/>
         <v>33.140283140283152</v>
       </c>
+      <c r="H351" s="25" t="s">
+        <v>1652</v>
+      </c>
       <c r="O351">
         <v>20170712</v>
       </c>
@@ -23151,7 +22758,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="355" spans="1:16" ht="27">
+    <row r="355" spans="1:16" ht="28.8">
       <c r="A355">
         <v>20190613</v>
       </c>
@@ -23164,8 +22771,8 @@
       <c r="D355" t="s">
         <v>1524</v>
       </c>
-      <c r="H355" s="16" t="s">
-        <v>1586</v>
+      <c r="H355" s="26" t="s">
+        <v>1653</v>
       </c>
       <c r="O355">
         <v>20170718</v>
@@ -23257,6 +22864,9 @@
         <f t="shared" si="14"/>
         <v>12.903225806451612</v>
       </c>
+      <c r="H359" s="25" t="s">
+        <v>1654</v>
+      </c>
       <c r="O359">
         <v>20170724</v>
       </c>
@@ -23299,8 +22909,8 @@
         <v>1530</v>
       </c>
       <c r="G361" s="4"/>
-      <c r="H361" s="15" t="s">
-        <v>1585</v>
+      <c r="H361" s="24" t="s">
+        <v>1655</v>
       </c>
       <c r="O361">
         <v>20170726</v>
@@ -23323,8 +22933,8 @@
         <v>1531</v>
       </c>
       <c r="G362" s="4"/>
-      <c r="H362" s="15" t="s">
-        <v>1583</v>
+      <c r="H362" s="24" t="s">
+        <v>1656</v>
       </c>
       <c r="O362">
         <v>20170727</v>
@@ -23347,8 +22957,8 @@
         <v>1532</v>
       </c>
       <c r="G363" s="4"/>
-      <c r="H363" s="15" t="s">
-        <v>1584</v>
+      <c r="H363" s="24" t="s">
+        <v>1657</v>
       </c>
       <c r="I363" s="6" t="s">
         <v>1560</v>
@@ -23374,8 +22984,8 @@
         <v>1533</v>
       </c>
       <c r="G364" s="4"/>
-      <c r="H364" s="15" t="s">
-        <v>1582</v>
+      <c r="H364" s="24" t="s">
+        <v>1661</v>
       </c>
       <c r="O364">
         <v>20170731</v>
@@ -23398,8 +23008,8 @@
         <v>1534</v>
       </c>
       <c r="G365" s="4"/>
-      <c r="H365" s="15" t="s">
-        <v>1581</v>
+      <c r="H365" s="24" t="s">
+        <v>1660</v>
       </c>
       <c r="O365">
         <v>20170801</v>
@@ -23422,8 +23032,8 @@
         <v>1535</v>
       </c>
       <c r="G366" s="4"/>
-      <c r="H366" s="15" t="s">
-        <v>1580</v>
+      <c r="H366" s="24" t="s">
+        <v>1659</v>
       </c>
       <c r="O366">
         <v>20170802</v>
@@ -23446,8 +23056,8 @@
         <v>1564</v>
       </c>
       <c r="G367" s="4"/>
-      <c r="H367" s="15" t="s">
-        <v>1579</v>
+      <c r="H367" s="24" t="s">
+        <v>1658</v>
       </c>
       <c r="O367">
         <v>20170803</v>
@@ -23470,8 +23080,8 @@
         <v>1536</v>
       </c>
       <c r="G368" s="4"/>
-      <c r="H368" s="15" t="s">
-        <v>1578</v>
+      <c r="H368" s="24" t="s">
+        <v>1662</v>
       </c>
       <c r="O368">
         <v>20170804</v>
@@ -23692,8 +23302,8 @@
         <f t="shared" si="14"/>
         <v>9.3939393939393963</v>
       </c>
-      <c r="H378" s="14" t="s">
-        <v>1588</v>
+      <c r="H378" s="25" t="s">
+        <v>1663</v>
       </c>
       <c r="O378">
         <v>20170818</v>
@@ -23737,8 +23347,8 @@
         <v>1548</v>
       </c>
       <c r="G380" s="6"/>
-      <c r="H380" s="15" t="s">
-        <v>1596</v>
+      <c r="H380" s="24" t="s">
+        <v>1664</v>
       </c>
       <c r="O380">
         <v>20170822</v>
@@ -23824,8 +23434,8 @@
         <v>1552</v>
       </c>
       <c r="G384" s="6"/>
-      <c r="H384" s="15" t="s">
-        <v>1576</v>
+      <c r="H384" s="24" t="s">
+        <v>1665</v>
       </c>
       <c r="O384">
         <v>20170828</v>
@@ -23848,8 +23458,8 @@
         <v>1553</v>
       </c>
       <c r="G385" s="6"/>
-      <c r="H385" s="15" t="s">
-        <v>1575</v>
+      <c r="H385" s="24" t="s">
+        <v>1666</v>
       </c>
       <c r="O385">
         <v>20170829</v>
@@ -23965,6 +23575,9 @@
         <f t="shared" si="14"/>
         <v>14.057507987220447</v>
       </c>
+      <c r="H390" s="25" t="s">
+        <v>1667</v>
+      </c>
       <c r="O390">
         <v>20170905</v>
       </c>
@@ -23983,7 +23596,7 @@
         <v>4</v>
       </c>
       <c r="D391" s="13" t="s">
-        <v>1633</v>
+        <v>1608</v>
       </c>
       <c r="E391">
         <v>8.99</v>
@@ -23995,6 +23608,9 @@
         <f t="shared" si="14"/>
         <v>-1.0011123470522787</v>
       </c>
+      <c r="H391" s="24" t="s">
+        <v>1644</v>
+      </c>
       <c r="O391">
         <v>20170906</v>
       </c>
@@ -24013,11 +23629,11 @@
         <v>6</v>
       </c>
       <c r="D392" s="13" t="s">
-        <v>1632</v>
+        <v>1607</v>
       </c>
       <c r="G392" s="13"/>
-      <c r="H392" s="15" t="s">
-        <v>1577</v>
+      <c r="H392" s="24" t="s">
+        <v>1668</v>
       </c>
       <c r="O392">
         <v>20170907</v>
@@ -24049,8 +23665,8 @@
         <f t="shared" ref="G393:G411" si="15">(F393-E393)/E393*100</f>
         <v>4.8412698412698365</v>
       </c>
-      <c r="H393" s="15" t="s">
-        <v>1574</v>
+      <c r="H393" s="25" t="s">
+        <v>1669</v>
       </c>
       <c r="O393">
         <v>20170908</v>
@@ -24103,6 +23719,9 @@
         <f t="shared" si="15"/>
         <v>-4.1424169804861375</v>
       </c>
+      <c r="H395" s="25" t="s">
+        <v>1652</v>
+      </c>
       <c r="O395">
         <v>20170912</v>
       </c>
@@ -24259,8 +23878,8 @@
         <f t="shared" si="15"/>
         <v>-7.1005917159763277</v>
       </c>
-      <c r="H402" s="14" t="s">
-        <v>1622</v>
+      <c r="H402" s="24" t="s">
+        <v>1670</v>
       </c>
       <c r="O402">
         <v>20170921</v>
@@ -24322,7 +23941,7 @@
         <v>8</v>
       </c>
       <c r="D405" s="13" t="s">
-        <v>1602</v>
+        <v>1578</v>
       </c>
       <c r="E405">
         <v>23.36</v>
@@ -24335,7 +23954,7 @@
         <v>19.306506849315074</v>
       </c>
       <c r="H405" s="14" t="s">
-        <v>1601</v>
+        <v>1577</v>
       </c>
       <c r="O405">
         <v>20170926</v>
@@ -24355,7 +23974,7 @@
         <v>11</v>
       </c>
       <c r="D406" s="13" t="s">
-        <v>1603</v>
+        <v>1579</v>
       </c>
       <c r="G406" s="13"/>
       <c r="O406">
@@ -24376,11 +23995,11 @@
         <v>16</v>
       </c>
       <c r="D407" s="13" t="s">
-        <v>1604</v>
+        <v>1580</v>
       </c>
       <c r="G407" s="13"/>
       <c r="H407" s="14" t="s">
-        <v>1600</v>
+        <v>1576</v>
       </c>
       <c r="O407">
         <v>20170928</v>
@@ -24400,7 +24019,7 @@
         <v>13</v>
       </c>
       <c r="D408" s="13" t="s">
-        <v>1605</v>
+        <v>1581</v>
       </c>
       <c r="E408">
         <v>8.56</v>
@@ -24430,7 +24049,7 @@
         <v>15</v>
       </c>
       <c r="D409" s="13" t="s">
-        <v>1606</v>
+        <v>1582</v>
       </c>
       <c r="G409" s="13"/>
       <c r="O409">
@@ -24451,7 +24070,7 @@
         <v>13</v>
       </c>
       <c r="D410" s="13" t="s">
-        <v>1607</v>
+        <v>1583</v>
       </c>
       <c r="G410" s="13"/>
       <c r="O410">
@@ -24472,7 +24091,7 @@
         <v>6</v>
       </c>
       <c r="D411" s="13" t="s">
-        <v>1608</v>
+        <v>1584</v>
       </c>
       <c r="E411">
         <v>4.2699999999999996</v>
@@ -24502,7 +24121,7 @@
         <v>11</v>
       </c>
       <c r="D412" s="13" t="s">
-        <v>1609</v>
+        <v>1585</v>
       </c>
       <c r="G412" s="13"/>
       <c r="O412">
@@ -24523,7 +24142,7 @@
         <v>15</v>
       </c>
       <c r="D413" s="13" t="s">
-        <v>1610</v>
+        <v>1586</v>
       </c>
       <c r="G413" s="13"/>
       <c r="O413">
@@ -24544,7 +24163,7 @@
         <v>12</v>
       </c>
       <c r="D414" s="13" t="s">
-        <v>1611</v>
+        <v>1587</v>
       </c>
       <c r="E414">
         <v>10.88</v>
@@ -24556,8 +24175,8 @@
         <f>(F414-E414)/E414*100</f>
         <v>3.8602941176470575</v>
       </c>
-      <c r="H414" s="13" t="s">
-        <v>1627</v>
+      <c r="H414" s="25" t="s">
+        <v>1602</v>
       </c>
       <c r="O414">
         <v>20171016</v>
@@ -24577,7 +24196,7 @@
         <v>11</v>
       </c>
       <c r="D415" s="13" t="s">
-        <v>1612</v>
+        <v>1588</v>
       </c>
       <c r="G415" s="13"/>
       <c r="O415">
@@ -24598,7 +24217,7 @@
         <v>9</v>
       </c>
       <c r="D416" s="13" t="s">
-        <v>1620</v>
+        <v>1596</v>
       </c>
       <c r="E416">
         <v>30.99</v>
@@ -24628,7 +24247,7 @@
         <v>15</v>
       </c>
       <c r="D417" s="13" t="s">
-        <v>1613</v>
+        <v>1589</v>
       </c>
       <c r="G417" s="13"/>
       <c r="O417">
@@ -24649,7 +24268,7 @@
         <v>16</v>
       </c>
       <c r="D418" s="13" t="s">
-        <v>1614</v>
+        <v>1590</v>
       </c>
       <c r="E418">
         <v>13.59</v>
@@ -24662,7 +24281,7 @@
         <v>-10.890360559234736</v>
       </c>
       <c r="H418" s="14" t="s">
-        <v>1625</v>
+        <v>1600</v>
       </c>
       <c r="O418">
         <v>20171020</v>
@@ -24682,7 +24301,7 @@
         <v>9</v>
       </c>
       <c r="D419" s="13" t="s">
-        <v>1615</v>
+        <v>1591</v>
       </c>
       <c r="E419">
         <v>9</v>
@@ -24695,7 +24314,7 @@
         <v>12.888888888888891</v>
       </c>
       <c r="H419" s="14" t="s">
-        <v>1624</v>
+        <v>1599</v>
       </c>
       <c r="O419">
         <v>20171023</v>
@@ -24715,7 +24334,7 @@
         <v>7</v>
       </c>
       <c r="D420" s="13" t="s">
-        <v>1616</v>
+        <v>1592</v>
       </c>
       <c r="E420">
         <v>12.5</v>
@@ -24728,7 +24347,7 @@
         <v>-14.560000000000004</v>
       </c>
       <c r="H420" s="14" t="s">
-        <v>1623</v>
+        <v>1598</v>
       </c>
       <c r="O420">
         <v>20171024</v>
@@ -24748,7 +24367,7 @@
         <v>10</v>
       </c>
       <c r="D421" s="13" t="s">
-        <v>1617</v>
+        <v>1593</v>
       </c>
       <c r="E421">
         <v>22</v>
@@ -24761,7 +24380,7 @@
         <v>-17.136363636363637</v>
       </c>
       <c r="H421" s="14" t="s">
-        <v>1626</v>
+        <v>1601</v>
       </c>
       <c r="O421">
         <v>20171025</v>
@@ -24781,7 +24400,7 @@
         <v>6</v>
       </c>
       <c r="D422" s="13" t="s">
-        <v>1618</v>
+        <v>1594</v>
       </c>
       <c r="G422" s="13"/>
       <c r="O422">
@@ -24802,7 +24421,7 @@
         <v>7</v>
       </c>
       <c r="D423" s="13" t="s">
-        <v>1619</v>
+        <v>1595</v>
       </c>
       <c r="E423">
         <v>28.61</v>
@@ -24814,8 +24433,8 @@
         <f t="shared" ref="G423:G427" si="17">(F423-E423)/E423*100</f>
         <v>28.940929744844464</v>
       </c>
-      <c r="H423" s="17" t="s">
-        <v>1621</v>
+      <c r="H423" s="16" t="s">
+        <v>1597</v>
       </c>
       <c r="O423">
         <v>20171027</v>
@@ -24835,9 +24454,9 @@
         <v>9</v>
       </c>
       <c r="D424" s="13" t="s">
-        <v>1628</v>
-      </c>
-      <c r="G424" s="19"/>
+        <v>1603</v>
+      </c>
+      <c r="G424" s="18"/>
       <c r="O424">
         <v>20171030</v>
       </c>
@@ -24856,9 +24475,9 @@
         <v>7</v>
       </c>
       <c r="D425" s="13" t="s">
-        <v>1629</v>
-      </c>
-      <c r="G425" s="19"/>
+        <v>1604</v>
+      </c>
+      <c r="G425" s="18"/>
       <c r="O425">
         <v>20171031</v>
       </c>
@@ -24877,11 +24496,11 @@
         <v>10</v>
       </c>
       <c r="D426" s="13" t="s">
-        <v>1630</v>
-      </c>
-      <c r="G426" s="19"/>
+        <v>1605</v>
+      </c>
+      <c r="G426" s="18"/>
       <c r="H426" s="15" t="s">
-        <v>1636</v>
+        <v>1611</v>
       </c>
       <c r="O426">
         <v>20171101</v>
@@ -24901,7 +24520,7 @@
         <v>10</v>
       </c>
       <c r="D427" s="13" t="s">
-        <v>1631</v>
+        <v>1606</v>
       </c>
       <c r="E427">
         <v>16</v>
@@ -24909,7 +24528,7 @@
       <c r="F427">
         <v>26.96</v>
       </c>
-      <c r="G427" s="19">
+      <c r="G427" s="18">
         <f t="shared" si="17"/>
         <v>68.5</v>
       </c>
@@ -24931,7 +24550,7 @@
         <v>6</v>
       </c>
       <c r="D428" s="13" t="s">
-        <v>1634</v>
+        <v>1609</v>
       </c>
       <c r="O428">
         <v>20171103</v>
@@ -24941,17 +24560,17 @@
       </c>
     </row>
     <row r="429" spans="1:16">
-      <c r="A429" s="18">
+      <c r="A429" s="17">
         <v>20190926</v>
       </c>
-      <c r="B429" s="18">
+      <c r="B429" s="17">
         <v>11</v>
       </c>
-      <c r="C429" s="18">
+      <c r="C429" s="17">
         <v>7</v>
       </c>
-      <c r="D429" s="19" t="s">
-        <v>1635</v>
+      <c r="D429" s="18" t="s">
+        <v>1610</v>
       </c>
       <c r="O429">
         <v>20171106</v>
@@ -24961,17 +24580,17 @@
       </c>
     </row>
     <row r="430" spans="1:16">
-      <c r="A430" s="18">
+      <c r="A430" s="17">
         <v>20190927</v>
       </c>
-      <c r="B430" s="18">
+      <c r="B430" s="17">
         <v>9</v>
       </c>
-      <c r="C430" s="18">
+      <c r="C430" s="17">
         <v>5</v>
       </c>
-      <c r="D430" s="19" t="s">
-        <v>1637</v>
+      <c r="D430" s="18" t="s">
+        <v>1612</v>
       </c>
       <c r="O430">
         <v>20171107</v>
@@ -24981,17 +24600,17 @@
       </c>
     </row>
     <row r="431" spans="1:16">
-      <c r="A431" s="18">
+      <c r="A431" s="17">
         <v>20190930</v>
       </c>
-      <c r="B431" s="18">
+      <c r="B431" s="17">
         <v>7</v>
       </c>
-      <c r="C431" s="18">
+      <c r="C431" s="17">
         <v>5</v>
       </c>
-      <c r="D431" s="19" t="s">
-        <v>1638</v>
+      <c r="D431" s="18" t="s">
+        <v>1613</v>
       </c>
       <c r="O431">
         <v>20171108</v>
@@ -25001,17 +24620,17 @@
       </c>
     </row>
     <row r="432" spans="1:16">
-      <c r="A432" s="18">
+      <c r="A432" s="17">
         <v>20191008</v>
       </c>
-      <c r="B432" s="18">
+      <c r="B432" s="17">
         <v>8</v>
       </c>
-      <c r="C432" s="18">
+      <c r="C432" s="17">
         <v>7</v>
       </c>
-      <c r="D432" s="19" t="s">
-        <v>1639</v>
+      <c r="D432" s="18" t="s">
+        <v>1614</v>
       </c>
       <c r="O432">
         <v>20171109</v>
@@ -25021,17 +24640,17 @@
       </c>
     </row>
     <row r="433" spans="1:16">
-      <c r="A433" s="18">
+      <c r="A433" s="17">
         <v>20191009</v>
       </c>
-      <c r="B433" s="18">
+      <c r="B433" s="17">
         <v>8</v>
       </c>
-      <c r="C433" s="18">
+      <c r="C433" s="17">
         <v>7</v>
       </c>
-      <c r="D433" s="19" t="s">
-        <v>1640</v>
+      <c r="D433" s="18" t="s">
+        <v>1615</v>
       </c>
       <c r="O433">
         <v>20171110</v>
@@ -25041,17 +24660,17 @@
       </c>
     </row>
     <row r="434" spans="1:16">
-      <c r="A434" s="18">
+      <c r="A434" s="17">
         <v>20191010</v>
       </c>
-      <c r="B434" s="18">
+      <c r="B434" s="17">
         <v>10</v>
       </c>
-      <c r="C434" s="18">
+      <c r="C434" s="17">
         <v>8</v>
       </c>
-      <c r="D434" s="19" t="s">
-        <v>1641</v>
+      <c r="D434" s="18" t="s">
+        <v>1616</v>
       </c>
       <c r="O434">
         <v>20171113</v>
@@ -25061,20 +24680,20 @@
       </c>
     </row>
     <row r="435" spans="1:16">
-      <c r="A435" s="21">
+      <c r="A435" s="20">
         <v>20191011</v>
       </c>
-      <c r="B435" s="21">
+      <c r="B435" s="20">
         <v>10</v>
       </c>
-      <c r="C435" s="21">
+      <c r="C435" s="20">
         <v>8</v>
       </c>
-      <c r="D435" s="22" t="s">
-        <v>1642</v>
-      </c>
-      <c r="H435" s="20" t="s">
-        <v>1646</v>
+      <c r="D435" s="21" t="s">
+        <v>1617</v>
+      </c>
+      <c r="H435" s="19" t="s">
+        <v>1626</v>
       </c>
       <c r="O435">
         <v>20171114</v>
@@ -25084,17 +24703,17 @@
       </c>
     </row>
     <row r="436" spans="1:16">
-      <c r="A436" s="21">
+      <c r="A436" s="20">
         <v>20191014</v>
       </c>
-      <c r="B436" s="21">
+      <c r="B436" s="20">
         <v>19</v>
       </c>
-      <c r="C436" s="21">
+      <c r="C436" s="20">
         <v>16</v>
       </c>
-      <c r="D436" s="22" t="s">
-        <v>1643</v>
+      <c r="D436" s="21" t="s">
+        <v>1618</v>
       </c>
       <c r="O436">
         <v>20171115</v>
@@ -25104,20 +24723,20 @@
       </c>
     </row>
     <row r="437" spans="1:16">
-      <c r="A437" s="21">
+      <c r="A437" s="20">
         <v>20191015</v>
       </c>
-      <c r="B437" s="21">
+      <c r="B437" s="20">
         <v>14</v>
       </c>
-      <c r="C437" s="21">
+      <c r="C437" s="20">
         <v>11</v>
       </c>
-      <c r="D437" s="22" t="s">
-        <v>1644</v>
-      </c>
-      <c r="H437" s="20" t="s">
-        <v>1646</v>
+      <c r="D437" s="21" t="s">
+        <v>1619</v>
+      </c>
+      <c r="H437" s="19" t="s">
+        <v>1621</v>
       </c>
       <c r="O437">
         <v>20171116</v>
@@ -25127,17 +24746,17 @@
       </c>
     </row>
     <row r="438" spans="1:16">
-      <c r="A438" s="23">
+      <c r="A438" s="22">
         <v>20191016</v>
       </c>
-      <c r="B438" s="23">
+      <c r="B438" s="22">
         <v>7</v>
       </c>
-      <c r="C438" s="23">
+      <c r="C438" s="22">
         <v>6</v>
       </c>
-      <c r="D438" s="24" t="s">
-        <v>1645</v>
+      <c r="D438" s="23" t="s">
+        <v>1620</v>
       </c>
       <c r="O438">
         <v>20171117</v>
@@ -25147,17 +24766,17 @@
       </c>
     </row>
     <row r="439" spans="1:16">
-      <c r="A439" s="23">
+      <c r="A439" s="22">
         <v>20191017</v>
       </c>
-      <c r="B439" s="23">
+      <c r="B439" s="22">
         <v>5</v>
       </c>
-      <c r="C439" s="23">
+      <c r="C439" s="22">
         <v>3</v>
       </c>
-      <c r="D439" s="24" t="s">
-        <v>1647</v>
+      <c r="D439" s="23" t="s">
+        <v>1622</v>
       </c>
       <c r="O439">
         <v>20171120</v>
@@ -25167,17 +24786,17 @@
       </c>
     </row>
     <row r="440" spans="1:16">
-      <c r="A440" s="23">
+      <c r="A440" s="22">
         <v>20191018</v>
       </c>
-      <c r="B440" s="23">
+      <c r="B440" s="22">
         <v>9</v>
       </c>
-      <c r="C440" s="23">
+      <c r="C440" s="22">
         <v>8</v>
       </c>
-      <c r="D440" s="24" t="s">
-        <v>1648</v>
+      <c r="D440" s="23" t="s">
+        <v>1623</v>
       </c>
       <c r="O440">
         <v>20171121</v>
@@ -25187,17 +24806,17 @@
       </c>
     </row>
     <row r="441" spans="1:16">
-      <c r="A441" s="23">
+      <c r="A441" s="22">
         <v>20191021</v>
       </c>
-      <c r="B441" s="23">
+      <c r="B441" s="22">
         <v>6</v>
       </c>
-      <c r="C441" s="23">
+      <c r="C441" s="22">
         <v>6</v>
       </c>
-      <c r="D441" s="24" t="s">
-        <v>1649</v>
+      <c r="D441" s="23" t="s">
+        <v>1624</v>
       </c>
       <c r="O441">
         <v>20171122</v>
@@ -25207,17 +24826,17 @@
       </c>
     </row>
     <row r="442" spans="1:16">
-      <c r="A442" s="23">
+      <c r="A442" s="22">
         <v>20191022</v>
       </c>
-      <c r="B442" s="23">
+      <c r="B442" s="22">
         <v>7</v>
       </c>
-      <c r="C442" s="23">
+      <c r="C442" s="22">
         <v>5</v>
       </c>
-      <c r="D442" s="24" t="s">
-        <v>1650</v>
+      <c r="D442" s="23" t="s">
+        <v>1625</v>
       </c>
       <c r="O442">
         <v>20171123</v>
@@ -25885,7 +25504,7 @@
       <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -27371,7 +26990,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -28873,7 +28492,7 @@
       <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -30819,7 +30438,7 @@
       <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -31569,7 +31188,7 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">

</xml_diff>